<commit_message>
parse opts from excel sheet, refine front-end app
</commit_message>
<xml_diff>
--- a/test/questions.xlsx
+++ b/test/questions.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Config" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Who is the McDonalds mascot?</t>
   </si>
@@ -82,6 +82,24 @@
   </si>
   <si>
     <t>Around</t>
+  </si>
+  <si>
+    <t>My derpy test</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>This description comes from the excel doc</t>
+  </si>
+  <si>
+    <t>randomizeQuestions</t>
+  </si>
+  <si>
+    <t>randomizeAnswers</t>
   </si>
 </sst>
 </file>
@@ -420,9 +438,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -573,18 +642,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>